<commit_message>
Corrected error in pbcore_instantiationphysicalaudio_vocabulary.xlsx and uploaded new version
The old version said "1/2 inch audio cassette" where it should have said "1/2 inch audio tape".
</commit_message>
<xml_diff>
--- a/assets/downloads/pbcore_instantiationphysicalaudio_vocabulary.xlsx
+++ b/assets/downloads/pbcore_instantiationphysicalaudio_vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sadie_roosa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owen_king\Desktop\pbcore_vocabs_XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6200F4A6-064D-DB47-8530-404848BC601C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ADDC13-23F9-488E-9A64-B610CAA4ED3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="25040" windowHeight="13740" xr2:uid="{70AE25B9-0A5B-AA45-A6C5-AF07CF7C892A}"/>
+    <workbookView xWindow="3510" yWindow="195" windowWidth="24915" windowHeight="15165" xr2:uid="{70AE25B9-0A5B-AA45-A6C5-AF07CF7C892A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>An open reel analog audiotape format.</t>
   </si>
   <si>
-    <t>1/2 inch audio cassette</t>
-  </si>
-  <si>
     <t>http://pbcore.org/pbcore-controlled-vocabularies/titletype-vocabulary/#HalfInchAudioTape</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>A wire-based magnetic analog audio format.</t>
+  </si>
+  <si>
+    <t>1/2 inch audio tape</t>
   </si>
 </sst>
 </file>
@@ -340,12 +340,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -663,18 +662,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0870A9B8-B6CC-1247-8DC9-8718523DCC82}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="60.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="60.375" customWidth="1"/>
     <col min="3" max="3" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,18 +684,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -707,7 +706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -718,359 +717,359 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="3"/>
     </row>
   </sheetData>

</xml_diff>